<commit_message>
added test script which proves and provides code for our goals
</commit_message>
<xml_diff>
--- a/testData/TestNames.xlsx
+++ b/testData/TestNames.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MengSpring\data-692\project\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MengSpring\data-692\project3\ENSF692-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B13A14F-BBA9-4828-A704-7D6F9C84A116}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08B7D8B-4F14-4D38-90D6-1374F5D1886F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="2730" windowWidth="21600" windowHeight="15585" xr2:uid="{A39412BA-4797-498C-B925-F034EBBE45B6}"/>
+    <workbookView xWindow="11745" yWindow="3195" windowWidth="21600" windowHeight="15585" xr2:uid="{A39412BA-4797-498C-B925-F034EBBE45B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>movie  ID</t>
-  </si>
-  <si>
     <t>title</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>The city of god</t>
+  </si>
+  <si>
+    <t>movie</t>
   </si>
 </sst>
 </file>
@@ -430,18 +430,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB866DCE-E701-473F-A9E2-A21458EE9FFC}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,7 +447,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -457,7 +455,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -465,7 +463,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -473,7 +471,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -481,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>